<commit_message>
Agregue Cuaderno a N6
</commit_message>
<xml_diff>
--- a/Calificaciones 2025-2026/N6_ENS_C.xlsx
+++ b/Calificaciones 2025-2026/N6_ENS_C.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GSE2GA\Documents\Personal\Tere Guerra\Meraki\N6_ENS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\activ\Documents\Meraki\Calificaciones 2025-2026\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920DDA8B-D8DB-4BCA-A7EB-F21145A8CA56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0B9B4B6-99DA-43B4-9343-4492CCA7C17F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-96" windowWidth="23256" windowHeight="12456" xr2:uid="{B2EF7373-A7E6-423B-9BCC-817B77FBEC7D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B2EF7373-A7E6-423B-9BCC-817B77FBEC7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Calificaciones" sheetId="3" r:id="rId1"/>
     <sheet name="Tareas" sheetId="1" r:id="rId2"/>
+    <sheet name="Cuaderno" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>No.</t>
   </si>
@@ -124,6 +125,15 @@
   </si>
   <si>
     <t>N6 PRIMARIA 6°A</t>
+  </si>
+  <si>
+    <t>Examen diagnóstico</t>
+  </si>
+  <si>
+    <t>Cuaderno</t>
+  </si>
+  <si>
+    <t>Actividad</t>
   </si>
 </sst>
 </file>
@@ -133,7 +143,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +153,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -246,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -277,10 +295,10 @@
     <xf numFmtId="164" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -292,6 +310,19 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -315,7 +346,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -633,11 +664,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AECF9521-3E5C-4485-A0EE-99CC705EEB69}">
   <dimension ref="B2:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
@@ -651,22 +682,22 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
@@ -876,7 +907,7 @@
       <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>0</v>
       </c>
       <c r="F9" s="9">
@@ -1104,10 +1135,10 @@
       <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="15">
-        <v>0</v>
-      </c>
-      <c r="F15" s="15">
+      <c r="E15" s="14">
+        <v>0</v>
+      </c>
+      <c r="F15" s="14">
         <v>0</v>
       </c>
       <c r="G15" s="9">
@@ -1229,7 +1260,7 @@
       <selection activeCell="W10" sqref="W10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="4.28515625" customWidth="1"/>
@@ -1243,29 +1274,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14" t="s">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
     </row>
     <row r="3" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
@@ -1405,7 +1436,7 @@
         <v>0</v>
       </c>
       <c r="T5" s="11">
-        <f>AVERAGE(E5:S5)</f>
+        <f t="shared" ref="T5:T15" si="0">AVERAGE(E5:S5)</f>
         <v>0</v>
       </c>
     </row>
@@ -1465,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="T6" s="11">
-        <f>AVERAGE(E6:S6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1525,7 +1556,7 @@
         <v>0</v>
       </c>
       <c r="T7" s="11">
-        <f>AVERAGE(E7:S7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1585,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="T8" s="11">
-        <f>AVERAGE(E8:S8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1645,7 +1676,7 @@
         <v>0</v>
       </c>
       <c r="T9" s="11">
-        <f>AVERAGE(E9:S9)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1705,7 +1736,7 @@
         <v>0</v>
       </c>
       <c r="T10" s="11">
-        <f>AVERAGE(E10:S10)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1765,7 +1796,7 @@
         <v>0</v>
       </c>
       <c r="T11" s="11">
-        <f>AVERAGE(E11:S11)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1825,7 +1856,7 @@
         <v>0</v>
       </c>
       <c r="T12" s="11">
-        <f>AVERAGE(E12:S12)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1885,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="T13" s="11">
-        <f>AVERAGE(E13:S13)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1945,7 +1976,7 @@
         <v>0</v>
       </c>
       <c r="T14" s="11">
-        <f>AVERAGE(E14:S14)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -2005,7 +2036,831 @@
         <v>0</v>
       </c>
       <c r="T15" s="11">
-        <f>AVERAGE(E15:S15)</f>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:T2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB897D3-7D3F-4CD4-94FB-95772F832F4F}">
+  <dimension ref="B2:Z16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Z5" sqref="Z5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="4.28515625" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="4.28515625" customWidth="1"/>
+    <col min="10" max="10" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="17" width="4.28515625" customWidth="1"/>
+    <col min="18" max="18" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="4.28515625" customWidth="1"/>
+    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+    </row>
+    <row r="3" spans="2:26" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
+      <c r="T3" s="8"/>
+    </row>
+    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="21">
+        <v>1</v>
+      </c>
+      <c r="F4" s="21">
+        <v>2</v>
+      </c>
+      <c r="G4" s="21">
+        <v>3</v>
+      </c>
+      <c r="H4" s="21">
+        <v>4</v>
+      </c>
+      <c r="I4" s="21">
+        <v>5</v>
+      </c>
+      <c r="J4" s="21">
+        <v>6</v>
+      </c>
+      <c r="K4" s="21">
+        <v>7</v>
+      </c>
+      <c r="L4" s="21">
+        <v>8</v>
+      </c>
+      <c r="M4" s="21">
+        <v>9</v>
+      </c>
+      <c r="N4" s="21">
+        <v>10</v>
+      </c>
+      <c r="O4" s="21">
+        <v>11</v>
+      </c>
+      <c r="P4" s="21">
+        <v>12</v>
+      </c>
+      <c r="Q4" s="21">
+        <v>13</v>
+      </c>
+      <c r="R4" s="21">
+        <v>14</v>
+      </c>
+      <c r="S4" s="21">
+        <v>15</v>
+      </c>
+      <c r="T4" s="21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="6"/>
+      <c r="Z5" s="23"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1044</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
+        <v>0</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0</v>
+      </c>
+      <c r="J6" s="10">
+        <v>0</v>
+      </c>
+      <c r="K6" s="10">
+        <v>0</v>
+      </c>
+      <c r="L6" s="10">
+        <v>0</v>
+      </c>
+      <c r="M6" s="10">
+        <v>0</v>
+      </c>
+      <c r="N6" s="10">
+        <v>0</v>
+      </c>
+      <c r="O6" s="10">
+        <v>0</v>
+      </c>
+      <c r="P6" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="10">
+        <v>0</v>
+      </c>
+      <c r="R6" s="10">
+        <v>0</v>
+      </c>
+      <c r="S6" s="10">
+        <v>0</v>
+      </c>
+      <c r="T6" s="11">
+        <f t="shared" ref="T6:T16" si="0">AVERAGE(E6:S6)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B7" s="5">
+        <v>2</v>
+      </c>
+      <c r="C7" s="5">
+        <v>879</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="10">
+        <v>0</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0</v>
+      </c>
+      <c r="K7" s="10">
+        <v>0</v>
+      </c>
+      <c r="L7" s="10">
+        <v>0</v>
+      </c>
+      <c r="M7" s="10">
+        <v>0</v>
+      </c>
+      <c r="N7" s="10">
+        <v>0</v>
+      </c>
+      <c r="O7" s="10">
+        <v>0</v>
+      </c>
+      <c r="P7" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="10">
+        <v>0</v>
+      </c>
+      <c r="R7" s="10">
+        <v>0</v>
+      </c>
+      <c r="S7" s="10">
+        <v>0</v>
+      </c>
+      <c r="T7" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B8" s="5">
+        <v>3</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1052</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0</v>
+      </c>
+      <c r="L8" s="10">
+        <v>0</v>
+      </c>
+      <c r="M8" s="10">
+        <v>0</v>
+      </c>
+      <c r="N8" s="10">
+        <v>0</v>
+      </c>
+      <c r="O8" s="10">
+        <v>0</v>
+      </c>
+      <c r="P8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>0</v>
+      </c>
+      <c r="R8" s="10">
+        <v>0</v>
+      </c>
+      <c r="S8" s="10">
+        <v>0</v>
+      </c>
+      <c r="T8" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B9" s="5">
+        <v>4</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1114</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0</v>
+      </c>
+      <c r="F9" s="10">
+        <v>0</v>
+      </c>
+      <c r="G9" s="10">
+        <v>0</v>
+      </c>
+      <c r="H9" s="10">
+        <v>0</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0</v>
+      </c>
+      <c r="J9" s="10">
+        <v>0</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0</v>
+      </c>
+      <c r="L9" s="10">
+        <v>0</v>
+      </c>
+      <c r="M9" s="10">
+        <v>0</v>
+      </c>
+      <c r="N9" s="10">
+        <v>0</v>
+      </c>
+      <c r="O9" s="10">
+        <v>0</v>
+      </c>
+      <c r="P9" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="10">
+        <v>0</v>
+      </c>
+      <c r="R9" s="10">
+        <v>0</v>
+      </c>
+      <c r="S9" s="10">
+        <v>0</v>
+      </c>
+      <c r="T9" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B10" s="5">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5">
+        <v>900</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0</v>
+      </c>
+      <c r="F10" s="10">
+        <v>0</v>
+      </c>
+      <c r="G10" s="10">
+        <v>0</v>
+      </c>
+      <c r="H10" s="10">
+        <v>0</v>
+      </c>
+      <c r="I10" s="10">
+        <v>0</v>
+      </c>
+      <c r="J10" s="10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="10">
+        <v>0</v>
+      </c>
+      <c r="L10" s="10">
+        <v>0</v>
+      </c>
+      <c r="M10" s="10">
+        <v>0</v>
+      </c>
+      <c r="N10" s="10">
+        <v>0</v>
+      </c>
+      <c r="O10" s="10">
+        <v>0</v>
+      </c>
+      <c r="P10" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>0</v>
+      </c>
+      <c r="R10" s="10">
+        <v>0</v>
+      </c>
+      <c r="S10" s="10">
+        <v>0</v>
+      </c>
+      <c r="T10" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B11" s="5">
+        <v>6</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1058</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0</v>
+      </c>
+      <c r="F11" s="10">
+        <v>0</v>
+      </c>
+      <c r="G11" s="10">
+        <v>0</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0</v>
+      </c>
+      <c r="K11" s="10">
+        <v>0</v>
+      </c>
+      <c r="L11" s="10">
+        <v>0</v>
+      </c>
+      <c r="M11" s="10">
+        <v>0</v>
+      </c>
+      <c r="N11" s="10">
+        <v>0</v>
+      </c>
+      <c r="O11" s="10">
+        <v>0</v>
+      </c>
+      <c r="P11" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>0</v>
+      </c>
+      <c r="R11" s="10">
+        <v>0</v>
+      </c>
+      <c r="S11" s="10">
+        <v>0</v>
+      </c>
+      <c r="T11" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B12" s="5">
+        <v>7</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1018</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0</v>
+      </c>
+      <c r="F12" s="10">
+        <v>0</v>
+      </c>
+      <c r="G12" s="10">
+        <v>0</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0</v>
+      </c>
+      <c r="J12" s="10">
+        <v>0</v>
+      </c>
+      <c r="K12" s="10">
+        <v>0</v>
+      </c>
+      <c r="L12" s="10">
+        <v>0</v>
+      </c>
+      <c r="M12" s="10">
+        <v>0</v>
+      </c>
+      <c r="N12" s="10">
+        <v>0</v>
+      </c>
+      <c r="O12" s="10">
+        <v>0</v>
+      </c>
+      <c r="P12" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>0</v>
+      </c>
+      <c r="R12" s="10">
+        <v>0</v>
+      </c>
+      <c r="S12" s="10">
+        <v>0</v>
+      </c>
+      <c r="T12" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B13" s="5">
+        <v>8</v>
+      </c>
+      <c r="C13" s="5">
+        <v>714</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0</v>
+      </c>
+      <c r="L13" s="10">
+        <v>0</v>
+      </c>
+      <c r="M13" s="10">
+        <v>0</v>
+      </c>
+      <c r="N13" s="10">
+        <v>0</v>
+      </c>
+      <c r="O13" s="10">
+        <v>0</v>
+      </c>
+      <c r="P13" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>0</v>
+      </c>
+      <c r="R13" s="10">
+        <v>0</v>
+      </c>
+      <c r="S13" s="10">
+        <v>0</v>
+      </c>
+      <c r="T13" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B14" s="5">
+        <v>9</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1010</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0</v>
+      </c>
+      <c r="F14" s="10">
+        <v>0</v>
+      </c>
+      <c r="G14" s="10">
+        <v>0</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0</v>
+      </c>
+      <c r="K14" s="10">
+        <v>0</v>
+      </c>
+      <c r="L14" s="10">
+        <v>0</v>
+      </c>
+      <c r="M14" s="10">
+        <v>0</v>
+      </c>
+      <c r="N14" s="10">
+        <v>0</v>
+      </c>
+      <c r="O14" s="10">
+        <v>0</v>
+      </c>
+      <c r="P14" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="10">
+        <v>0</v>
+      </c>
+      <c r="R14" s="10">
+        <v>0</v>
+      </c>
+      <c r="S14" s="10">
+        <v>0</v>
+      </c>
+      <c r="T14" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B15" s="5">
+        <v>10</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1211</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0</v>
+      </c>
+      <c r="F15" s="10">
+        <v>0</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0</v>
+      </c>
+      <c r="J15" s="10">
+        <v>0</v>
+      </c>
+      <c r="K15" s="10">
+        <v>0</v>
+      </c>
+      <c r="L15" s="10">
+        <v>0</v>
+      </c>
+      <c r="M15" s="10">
+        <v>0</v>
+      </c>
+      <c r="N15" s="10">
+        <v>0</v>
+      </c>
+      <c r="O15" s="10">
+        <v>0</v>
+      </c>
+      <c r="P15" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="10">
+        <v>0</v>
+      </c>
+      <c r="R15" s="10">
+        <v>0</v>
+      </c>
+      <c r="S15" s="10">
+        <v>0</v>
+      </c>
+      <c r="T15" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+      <c r="B16" s="5">
+        <v>11</v>
+      </c>
+      <c r="C16" s="5">
+        <v>880</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0</v>
+      </c>
+      <c r="F16" s="10">
+        <v>0</v>
+      </c>
+      <c r="G16" s="10">
+        <v>0</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0</v>
+      </c>
+      <c r="I16" s="10">
+        <v>0</v>
+      </c>
+      <c r="J16" s="10">
+        <v>0</v>
+      </c>
+      <c r="K16" s="10">
+        <v>0</v>
+      </c>
+      <c r="L16" s="10">
+        <v>0</v>
+      </c>
+      <c r="M16" s="10">
+        <v>0</v>
+      </c>
+      <c r="N16" s="10">
+        <v>0</v>
+      </c>
+      <c r="O16" s="10">
+        <v>0</v>
+      </c>
+      <c r="P16" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="10">
+        <v>0</v>
+      </c>
+      <c r="R16" s="10">
+        <v>0</v>
+      </c>
+      <c r="S16" s="10">
+        <v>0</v>
+      </c>
+      <c r="T16" s="11">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>